<commit_message>
Deleted theme settings to show category description.
</commit_message>
<xml_diff>
--- a/PairWise - категория, Сетка.xlsx
+++ b/PairWise - категория, Сетка.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
   <si>
     <t xml:space="preserve">Страница категории “Сетка”</t>
   </si>
@@ -92,51 +92,39 @@
     <t xml:space="preserve">Настройки темы</t>
   </si>
   <si>
-    <t xml:space="preserve">Show subcategories on category pages </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display category description </t>
-  </si>
-  <si>
-    <t xml:space="preserve">After products </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Before products </t>
+    <t xml:space="preserve">Decolorize out of stock products </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price display format </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show price at the top </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display empty stars of product rating </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display common value of product rating </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of lines in the product name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show product code (Sku) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display availability status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show quantity changer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show "Add to Cart" button </t>
   </si>
   <si>
     <t xml:space="preserve">Don't display </t>
   </si>
   <si>
-    <t xml:space="preserve">Decolorize out of stock products </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price display format </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show price at the top </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display empty stars of product rating </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display common value of product rating </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of lines in the product name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show product code (Sku) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display availability status </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show quantity changer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show "Add to Cart" button </t>
-  </si>
-  <si>
     <t xml:space="preserve">Icon of the Cart only (simplified version) </t>
   </si>
   <si>
@@ -288,15 +276,6 @@
   </si>
   <si>
     <t xml:space="preserve">Коды настроек темы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DCD_After</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DCD_Before</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThemeProductLists_DCD_Dont</t>
   </si>
   <si>
     <t xml:space="preserve">ThemeProductLists_DOOSP_On</t>
@@ -534,19 +513,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -673,418 +652,393 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="0" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="0" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" s="3" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>8</v>
+      <c r="D28" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D29" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+    <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="3" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="3" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="C34" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="0" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1103,354 +1057,340 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="33.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="0" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="0" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="0" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="0" t="s">
+    <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="0" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="F22" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="G22" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="0" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="0" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="0" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G23" s="0" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="0" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use another category "HTC"
</commit_message>
<xml_diff>
--- a/PairWise - категория, Сетка.xlsx
+++ b/PairWise - категория, Сетка.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Перечень настроек" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Настройки и Условия" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Коды значений" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="129">
   <si>
     <t xml:space="preserve">Страница категории “Сетка”</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t xml:space="preserve">Условия подготовки:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Категории добавить описание</t>
   </si>
   <si>
     <t xml:space="preserve">В категории должен быть товар без наличия</t>
@@ -652,10 +649,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1002,12 +999,12 @@
       <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C33" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1034,11 +1031,6 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1059,7 +1051,7 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1076,7 +1068,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,13 +1076,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,10 +1090,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,10 +1101,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1120,13 +1112,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,10 +1126,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,10 +1137,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,10 +1148,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,15 +1159,15 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,10 +1175,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1194,16 +1186,16 @@
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,10 +1203,10 @@
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,10 +1214,10 @@
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,10 +1225,10 @@
         <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,16 +1236,16 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,10 +1253,10 @@
         <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,10 +1264,10 @@
         <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1283,10 +1275,10 @@
         <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,19 +1286,19 @@
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,22 +1306,22 @@
         <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1337,10 +1329,10 @@
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1348,10 +1340,10 @@
         <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,10 +1351,10 @@
         <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,13 +1362,13 @@
         <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,13 +1376,13 @@
         <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test-case "TestCase01_CategoryPage_GridTest" is totally ready!
</commit_message>
<xml_diff>
--- a/PairWise - категория, Сетка.xlsx
+++ b/PairWise - категория, Сетка.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="128">
   <si>
     <t xml:space="preserve">Страница категории “Сетка”</t>
   </si>
@@ -191,28 +191,25 @@
     <t xml:space="preserve">Условия подготовки:</t>
   </si>
   <si>
-    <t xml:space="preserve">В категории должен быть товар без наличия</t>
+    <t xml:space="preserve">Товар без наличия</t>
   </si>
   <si>
     <t xml:space="preserve">все эти товары можно взять из категории HTC и работать только с этой категорией</t>
   </si>
   <si>
-    <t xml:space="preserve">В категории должен быть товар без наличия и с действием</t>
-  </si>
-  <si>
-    <t xml:space="preserve">В категории должен быть товар без изображений</t>
-  </si>
-  <si>
-    <t xml:space="preserve">В категории должен быть товар без цены</t>
-  </si>
-  <si>
-    <t xml:space="preserve">В категории должен быть товар без цены и с действием </t>
+    <t xml:space="preserve">Товар без наличия и с действием “Предзаказ”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Товар без цены</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Товар без цены и с действием “Попросить покупателя ввести цену”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Товар со скидкой</t>
   </si>
   <si>
     <t xml:space="preserve">Подготовить бренд — вывод логотипа на стр категории</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Товар со скидкой</t>
   </si>
   <si>
     <t xml:space="preserve">Коды цветосхемы</t>
@@ -652,7 +649,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1029,9 +1026,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A39" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1068,7 +1063,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,13 +1071,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,10 +1085,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1101,10 +1096,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,13 +1107,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,10 +1121,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,10 +1132,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1148,10 +1143,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,15 +1154,15 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,10 +1170,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,16 +1181,16 @@
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,10 +1198,10 @@
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,10 +1209,10 @@
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,10 +1220,10 @@
         <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1236,16 +1231,16 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,10 +1248,10 @@
         <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,10 +1259,10 @@
         <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,10 +1270,10 @@
         <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,19 +1281,19 @@
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1306,22 +1301,22 @@
         <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,10 +1324,10 @@
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1340,10 +1335,10 @@
         <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1351,10 +1346,10 @@
         <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1362,13 +1357,13 @@
         <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,13 +1371,13 @@
         <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>